<commit_message>
Update LAFPC Data Resource List.xlsx
</commit_message>
<xml_diff>
--- a/LAFPC Data Resource List.xlsx
+++ b/LAFPC Data Resource List.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chesneymelissinos/Desktop/Coding/lafpc/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22AF992-FE81-504C-AEA1-3534E2DDEF2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Resource List" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Suggestions for Future Research" sheetId="2" r:id="rId5"/>
+    <sheet name="Resource List" sheetId="1" r:id="rId1"/>
+    <sheet name="Suggestions for Future Research" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
   <si>
     <t>Source</t>
   </si>
@@ -28,17 +37,19 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>US Census Quickfacts</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
+        <u/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
-        <u/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (state, county, city, zip code)</t>
     </r>
@@ -60,14 +71,18 @@
   <si>
     <r>
       <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>American Community Survey (ACS)</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <color rgb="FF000000"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (state, county, census tract, zip code)</t>
     </r>
@@ -86,13 +101,20 @@
   <si>
     <r>
       <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>CalFresh Data Dashboard</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> (state, county)</t>
     </r>
   </si>
@@ -122,13 +144,20 @@
   <si>
     <r>
       <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>List of Farmers Markets</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> (county)</t>
     </r>
   </si>
@@ -141,13 +170,20 @@
   <si>
     <r>
       <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Food Assistance Providers Map</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> (county, service planning area)</t>
     </r>
   </si>
@@ -161,14 +197,16 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>USDA Food Atlas</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (state, county)</t>
@@ -191,17 +229,19 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Food Finder Map</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
+        <u/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
-        <u/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (county, city, neighborhood)</t>
     </r>
@@ -221,17 +261,19 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>List of Grocery Stores</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
+        <u/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
-        <u/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (city)</t>
     </r>
@@ -242,16 +284,18 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>List of Food Resources</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (city)</t>
     </r>
@@ -265,17 +309,19 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Equity Explorer Map</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
+        <u/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
-        <u/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (county, city, supervisorial district, neighborhood)</t>
     </r>
@@ -302,17 +348,19 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>ARPA Projects Map</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
+        <u/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
-        <u/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (county, supervisorial district)</t>
     </r>
@@ -334,14 +382,18 @@
   <si>
     <r>
       <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Census Reporter</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <color rgb="FF000000"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (state, county, city, congressional district, census tract)</t>
     </r>
@@ -360,13 +412,20 @@
   <si>
     <r>
       <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Neighborhood Data for Social Change</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> (city, census tract, neighborhood)</t>
     </r>
   </si>
@@ -388,13 +447,20 @@
   <si>
     <r>
       <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Number of Food Outlets Map</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> (county, census tract)</t>
     </r>
   </si>
@@ -404,14 +470,18 @@
   <si>
     <r>
       <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Food Desert and Food Assistance Desert Map</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
         <color rgb="FF000000"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> (census tract, service planning area)</t>
     </r>
@@ -442,85 +512,195 @@
   </si>
   <si>
     <t>List of number/names of convenience/liquor stores</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Income/Poverty</t>
+  </si>
+  <si>
+    <t>CalFresh Users, CalFresh Data</t>
+  </si>
+  <si>
+    <t>Race/Ethnicity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farmers' Markets, </t>
+  </si>
+  <si>
+    <t>Food Distribution, Food Banks, Food Panties</t>
+  </si>
+  <si>
+    <t>Children/Youth, Farmers' Markets, Grocery Stores, Seniors, Food Benefit, Food Pantries</t>
+  </si>
+  <si>
+    <t>Food Distribution, Income/Poverty, Seniors, Grocery Stores</t>
+  </si>
+  <si>
+    <t>Race/Ethnicity, Sex, Age</t>
+  </si>
+  <si>
+    <t>Food Distribution</t>
+  </si>
+  <si>
+    <t>Food Deserts, Food Assistance</t>
+  </si>
+  <si>
+    <t>Level of Education, Income/Poverty, Health</t>
+  </si>
+  <si>
+    <t>Race/Ethnicity, Sex, Age, Place of Origin, Level of Education, Income/Poverty, Health</t>
+  </si>
+  <si>
+    <t>Place of Origin, Poverty/Income, Level of Education, Health</t>
+  </si>
+  <si>
+    <t>Level of Education, Income/Poverty, Food Insecurity, Health</t>
+  </si>
+  <si>
+    <t>Grocery Stores, Restaurants</t>
+  </si>
+  <si>
+    <t>Grocery Stores, Restaurants, Farmers' Markets, Income/Poverty, Food Insecurity, Health</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="15">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -528,7 +708,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -538,102 +718,93 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="28">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -823,25 +994,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="65.5"/>
-    <col customWidth="1" min="2" max="2" width="68.25"/>
-    <col customWidth="1" min="3" max="3" width="43.0"/>
+    <col min="1" max="1" width="65.5" customWidth="1"/>
+    <col min="2" max="2" width="57.6640625" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -851,294 +1028,351 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="D1" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="21"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3"/>
-    </row>
-    <row r="3">
+      <c r="E2" s="23"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="D3" s="23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="D4" s="23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
+      <c r="D5" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="10" t="s">
+      <c r="D6" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="D7" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="11" t="s">
+      <c r="D8" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="D9" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="12" t="s">
+      <c r="D10" s="23"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="13"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="14" t="s">
+      <c r="B11" s="11"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="15" t="s">
+      <c r="D12" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="27" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="17" t="s">
+      <c r="D13" s="23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="D14" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-    </row>
-    <row r="16">
+      <c r="D15" s="23"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17">
+      <c r="D16" s="23"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="18" t="s">
+      <c r="D17" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="19"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="19" t="s">
+      <c r="D18" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="17"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="7" t="s">
+      <c r="D21" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="10" t="s">
+      <c r="D22" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="19" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="10" t="s">
+      <c r="D23" s="23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="26" t="s">
         <v>49</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25">
+      <c r="D24" s="23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A3"/>
-    <hyperlink r:id="rId2" ref="A4"/>
-    <hyperlink r:id="rId3" ref="A5"/>
-    <hyperlink r:id="rId4" ref="A6"/>
-    <hyperlink r:id="rId5" ref="A7"/>
-    <hyperlink r:id="rId6" ref="A8"/>
-    <hyperlink r:id="rId7" ref="A9"/>
-    <hyperlink r:id="rId8" ref="A12"/>
-    <hyperlink r:id="rId9" ref="A13"/>
-    <hyperlink r:id="rId10" ref="A14"/>
-    <hyperlink r:id="rId11" ref="A17"/>
-    <hyperlink r:id="rId12" ref="A18"/>
-    <hyperlink r:id="rId13" ref="A21"/>
-    <hyperlink r:id="rId14" ref="A22"/>
-    <hyperlink r:id="rId15" ref="A23"/>
-    <hyperlink r:id="rId16" ref="A24"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A17" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A18" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A23" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
   </hyperlinks>
-  <drawing r:id="rId17"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="76.0"/>
+    <col min="1" max="1" width="76" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="11" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>